<commit_message>
Added to sup mat
Also added some new plots
</commit_message>
<xml_diff>
--- a/Analyses/Experiment_4_Prob/Keep track.xlsx
+++ b/Analyses/Experiment_4_Prob/Keep track.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni\Github\Breaking_symmetry\Analyses\Experiment_4_Prob\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64217C4A-E22A-48B0-996A-D22709776C57}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512EE16C-40F0-418E-942D-C5D1DF75CEF5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="4890" xr2:uid="{CEE157A5-D3F9-4D8C-89DD-F8EBCCA79F21}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{CEE157A5-D3F9-4D8C-89DD-F8EBCCA79F21}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
     <t>M</t>
   </si>
   <si>
-    <t>Exclude</t>
+    <t>Include</t>
   </si>
 </sst>
 </file>
@@ -403,7 +403,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +449,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -469,7 +469,7 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -489,7 +489,7 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -509,7 +509,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -569,7 +569,7 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -589,7 +589,7 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -649,7 +649,7 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,7 +689,7 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -709,7 +709,7 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -729,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -749,7 +749,7 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -769,7 +769,7 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -789,7 +789,7 @@
         <v>2</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -809,7 +809,7 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>